<commit_message>
unhide columns, update fields
</commit_message>
<xml_diff>
--- a/templates/data-templates/2020-11_data_occurrence.xlsx
+++ b/templates/data-templates/2020-11_data_occurrence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biodiversityaq/Desktop/data-mgt-templates/templates/data-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A889B96-642B-4E4F-9B8D-27C2ECF49508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D521F8FE-C18F-F041-B3BD-A2C9B693193E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="occurrence" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
-  <si>
-    <t>Field</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>occurrenceID</t>
   </si>
@@ -82,9 +79,6 @@
     <t>day</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>timeZone</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
   </si>
   <si>
     <t xml:space="preserve"> occurrenceStatus</t>
-  </si>
-  <si>
-    <t>individualcount</t>
   </si>
   <si>
     <t>organismQuantity</t>
@@ -115,9 +106,6 @@
     <t>occurrenceRemarks</t>
   </si>
   <si>
-    <t>identifiedBy</t>
-  </si>
-  <si>
     <t>dateIdentified</t>
   </si>
   <si>
@@ -131,9 +119,6 @@
   </si>
   <si>
     <t>kingdom</t>
-  </si>
-  <si>
-    <t>taxonrank</t>
   </si>
   <si>
     <t>scientificNameID</t>
@@ -159,14 +144,33 @@
   <si>
     <t>Occurrence</t>
   </si>
+  <si>
+    <t>identifiedByID</t>
+  </si>
+  <si>
+    <t>individualCount</t>
+  </si>
+  <si>
+    <t>eventTime</t>
+  </si>
+  <si>
+    <t>taxonRank</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -261,25 +265,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,49 +602,49 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="127" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22" style="2"/>
-    <col min="3" max="5" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="2"/>
-    <col min="7" max="9" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="22" style="2"/>
-    <col min="12" max="12" width="22" style="2" customWidth="1"/>
-    <col min="13" max="13" width="22" style="2"/>
-    <col min="14" max="19" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="22" style="2"/>
-    <col min="21" max="29" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="22" style="2"/>
-    <col min="31" max="34" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="35" max="16384" width="22" style="2"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="4" width="22" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="2" customWidth="1"/>
+    <col min="6" max="8" width="22" style="2" customWidth="1"/>
+    <col min="9" max="10" width="22" style="2"/>
+    <col min="11" max="11" width="22" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22" style="2"/>
+    <col min="13" max="18" width="22" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22" style="2"/>
+    <col min="20" max="28" width="22" style="2" customWidth="1"/>
+    <col min="29" max="29" width="22" style="2"/>
+    <col min="30" max="33" width="22" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="22" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:36" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
@@ -648,16 +653,16 @@
       <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="7" t="s">
@@ -667,70 +672,67 @@
         <v>14</v>
       </c>
       <c r="P1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="V1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="W1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AC1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AD1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AE1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AF1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AG1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -767,16 +769,15 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
       <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{A5BDB4E7-DFB2-D747-98D2-42238535B471}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{A5BDB4E7-DFB2-D747-98D2-42238535B471}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{13198139-C46C-6E47-950B-E9FD90367D7F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{13198139-C46C-6E47-950B-E9FD90367D7F}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
@@ -790,7 +791,7 @@
           <x14:formula1>
             <xm:f>vocabulary!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -802,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C194D03-462E-F34B-9E67-653E278CCA9A}">
   <dimension ref="A1:A16384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -813,42 +814,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">

</xml_diff>